<commit_message>
Add new branch remotely from local
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Language</t>
   </si>
@@ -63,131 +63,183 @@
     <t>basic command</t>
   </si>
   <si>
-    <t>git checkout {branch name or hashcode}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>checkout</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Git</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>git branch</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>list all branch</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>git branch new_branch</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>create branch</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>update remote repo or update local repo</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Git</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>git push origin master 
-git pull origin master</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete  branch</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>git branch -d new_branch</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>git log --graph --oneline --decorate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Git</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>graph</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>merge</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Git</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. as long as the changed files are different between 2 branch, merge can go fast-forward wo additional modificaiton
-2. git merge branch-bug-fix</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>remote ops</t>
   </si>
   <si>
     <t>$git rm {file}
 $git status (-s)
 $git diff
 $git diff --cached</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>checkout</t>
+  </si>
+  <si>
+    <t>git checkout {branch name or hashcode}</t>
+  </si>
+  <si>
+    <t>list all branch</t>
+  </si>
+  <si>
+    <t>git branch</t>
+  </si>
+  <si>
+    <t>create branch</t>
+  </si>
+  <si>
+    <t>git branch new_branch</t>
+  </si>
+  <si>
+    <t>delete  branch</t>
+  </si>
+  <si>
+    <t>git branch -d new_branch</t>
+  </si>
+  <si>
+    <t>update remote repo or update local repo</t>
+  </si>
+  <si>
+    <t>git push origin master 
+git pull origin master</t>
+  </si>
+  <si>
+    <t>graph</t>
+  </si>
+  <si>
+    <t>git log --graph --oneline --decorate</t>
+  </si>
+  <si>
+    <t>merge</t>
+  </si>
+  <si>
+    <t>1. as long as the changed files are different between 2 branch, merge can go fast-forward wo additional modificaiton
+2. git merge branch-bug-fix</t>
   </si>
   <si>
     <t>diff</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Git</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>When you have staged all your new files, you can use below command to compare the difference to last commit:
 &gt;git diff --cached</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">$git remote show     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+origin
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">$git remote -v </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">          
+origin https://github…library.git (fetch)
+origin https://github…library.git (push)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$ git remote add pb https://github.com/paulboone/ticgit
+$ git remote -v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+origin https://github.com/schacon/ticgit (fetch)
+origin https://github.com/schacon/ticgit (push)
+pb https://github.com/paulboone/ticgit (fetch)
+pb https://github.com/paulboone/ticgit (push)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -217,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -229,9 +281,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -244,7 +300,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -318,7 +374,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -353,7 +408,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -529,21 +583,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
-    <col min="2" max="2" width="17.25" customWidth="1"/>
-    <col min="3" max="3" width="72.75" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="72.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,159 +608,167 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="38.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="46.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:3" ht="51.75">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="141">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="26.25">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="39">
+      <c r="A12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="39">
+      <c r="A13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="141">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="126" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -714,12 +776,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add git remote branch entry
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Language</t>
   </si>
@@ -63,9 +63,6 @@
     <t>basic command</t>
   </si>
   <si>
-    <t>remote ops</t>
-  </si>
-  <si>
     <t>$git rm {file}
 $git status (-s)
 $git diff
@@ -123,6 +120,81 @@
 &gt;git diff --cached</t>
   </si>
   <si>
+    <t>remote basic</t>
+  </si>
+  <si>
+    <t>remote branch</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">$ git branch -r </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+origin/HEAD -&gt; origin/master
+origin/master
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">$ git push origin master:new_branch //Crt new brnch on rmt &amp; push lcl/mstr to it
+$ git branch -r </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+origin/HEAD -&gt; origin/master
+origin/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>new_branch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+origin/master</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -190,8 +262,48 @@
       <t xml:space="preserve">
 origin https://github.com/schacon/ticgit (fetch)
 origin https://github.com/schacon/ticgit (push)
-pb https://github.com/paulboone/ticgit (fetch)
-pb https://github.com/paulboone/ticgit (push)</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">pb </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">https://github.com/paulboone/ticgit (fetch)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">pb </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://github.com/paulboone/ticgit (push)</t>
     </r>
   </si>
 </sst>
@@ -199,7 +311,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +354,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -269,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -278,9 +397,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -586,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,151 +725,158 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" ht="38.25">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51.75">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="141">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="141">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6" t="s">
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="6" t="s">
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="6" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="26.25">
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="26.25">
-      <c r="A10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="6" t="s">
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="6" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="39">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="39">
-      <c r="A12" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="6" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="39">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="39">
-      <c r="A13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="6" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="141">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="141">
-      <c r="A14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="102.75">
+      <c r="A15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="C15" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Add git diff usage
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Language</t>
   </si>
@@ -152,11 +152,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>When you have staged all your new files, you can use below command to compare the difference to last commit:
-&gt;git diff --cached</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>當你不想要一些unstaged changes時</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -182,7 +177,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -192,7 +187,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -204,7 +199,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -214,7 +209,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -227,7 +222,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -238,7 +233,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -251,7 +246,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -261,7 +256,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -272,7 +267,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -282,7 +277,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -297,7 +292,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -307,7 +302,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -320,7 +315,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -331,7 +326,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -343,7 +338,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -353,44 +348,55 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
 origin/master</t>
     </r>
+  </si>
+  <si>
+    <t>When you have staged all your new files, you can use below command to compare the difference to last commit:
+&gt;git diff --cached</t>
+  </si>
+  <si>
+    <t>diff of a file between commits</t>
+  </si>
+  <si>
+    <t>git diff &lt;revision_1&gt;:&lt;file_1&gt; &lt;revision_2&gt;:&lt;file_2&gt;
+for example: git diff master:pom.xml d44ac61:pom.xml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -398,21 +404,21 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="4"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -458,7 +464,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -471,7 +477,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -545,7 +551,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -580,7 +585,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -756,21 +760,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
-    <col min="2" max="2" width="17.25" customWidth="1"/>
-    <col min="3" max="3" width="72.75" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="72.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -781,7 +785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="38.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -792,7 +796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="51.75">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -803,7 +807,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -814,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="141">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -825,7 +829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -836,7 +840,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -847,7 +851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -858,7 +862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -869,7 +873,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="26.25">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
@@ -880,7 +884,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -891,7 +895,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="39">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -902,7 +906,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="39">
       <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
@@ -910,40 +914,51 @@
         <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="26.25">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="90">
+      <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="5" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="141">
+      <c r="A16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="C16" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="102.75">
+      <c r="A17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="111" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -953,12 +968,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -966,12 +981,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add man page of netcat and nmap, add entry into git.xls
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Language</t>
   </si>
@@ -366,6 +366,99 @@
   <si>
     <t>git diff &lt;revision_1&gt;:&lt;file_1&gt; &lt;revision_2&gt;:&lt;file_2&gt;
 for example: git diff master:pom.xml d44ac61:pom.xml</t>
+  </si>
+  <si>
+    <t>tricks abt revisioning</t>
+  </si>
+  <si>
+    <r>
+      <t>$ git show {branch_name/at_least_4_digit_of_commit_SHA1} //show certain commit diff compare to last commit
+$ git reflog //system will name the log in format HEAD@{n} so you can easily ref them
+$ git show {branch_name/at_least_4_digit_of_commit_SHA1}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  //show previous commit
+$ git show {branch_name/at_least_4_digit_of_commit_SHA1}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>^2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  //show 2nd parent (only for merge commit)
+$ git show {branch_name/at_least_4_digit_of_commit_SHA1}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>^^^...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> //show previous n generation father
+$ git show {branch_name/at_least_4_digit_of_commit_SHA1}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>~n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> //equivalent to last command</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -761,17 +854,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="72.7109375" customWidth="1"/>
+    <col min="3" max="3" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -961,9 +1054,144 @@
         <v>38</v>
       </c>
     </row>
+    <row r="18" spans="1:3" ht="128.25">
+      <c r="A18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add git library entry on how to solve local/remote conflict
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>Language</t>
   </si>
@@ -177,7 +177,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -187,7 +187,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -199,7 +199,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -209,7 +209,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -222,7 +222,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -233,7 +233,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -246,7 +246,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -256,7 +256,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -267,7 +267,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -277,7 +277,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -292,7 +292,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -302,7 +302,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -315,7 +315,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -326,7 +326,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -338,7 +338,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -348,7 +348,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -380,7 +380,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -390,7 +390,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -401,7 +401,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -411,7 +411,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -422,7 +422,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -432,7 +432,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -443,7 +443,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -453,43 +453,72 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> //equivalent to last command</t>
     </r>
+  </si>
+  <si>
+    <t>Master trapped in a wrong commit tunnel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remote</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Force-push from local to remote</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ git push -f {target_branch_like_origin} {new_of_local_branch}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. First of all, assume the wrong tunnel commit cannot/shouldnot merge to head, so steps would be delete the master branch first, and then re-create master branch at the right commit
+$ git checkout master
+$ git branch wrong_track &amp;&amp; git checkout wrong_track  &lt;--- cannot delete master when using it
+$ git branch -d master
+$ git checkout {master_or_any_other_commit}
+$ git branch master</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -497,21 +526,21 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="4"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -557,7 +586,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -570,7 +599,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -644,6 +673,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -678,6 +708,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -853,21 +884,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="74.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="17.25" customWidth="1"/>
+    <col min="3" max="3" width="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -878,7 +909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="38.25">
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -889,7 +920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="51.75">
+    <row r="3" spans="1:3" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -900,7 +931,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -911,7 +942,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="141">
+    <row r="5" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -922,7 +953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -933,7 +964,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -944,7 +975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -955,7 +986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -966,7 +997,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="26.25">
+    <row r="10" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
@@ -977,7 +1008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -988,7 +1019,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="39">
+    <row r="12" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -999,7 +1030,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="39">
+    <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
@@ -1010,7 +1041,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="26.25">
+    <row r="14" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1052,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="90">
+    <row r="15" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
@@ -1032,9 +1063,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="141">
+    <row r="16" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>35</v>
@@ -1043,9 +1074,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="102.75">
+    <row r="17" spans="1:3" ht="111" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>37</v>
@@ -1054,9 +1085,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="128.25">
+    <row r="18" spans="1:3" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>42</v>
@@ -1065,127 +1096,139 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3">
+    <row r="19" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
     </row>
   </sheetData>
@@ -1196,12 +1239,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1209,12 +1252,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add git entry talks about using a local folder as "remote repo"
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Language</t>
   </si>
@@ -177,7 +177,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -187,7 +187,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -199,7 +199,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -209,7 +209,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -222,7 +222,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -233,7 +233,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -246,7 +246,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -256,7 +256,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -267,7 +267,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -277,7 +277,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -292,7 +292,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -302,7 +302,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -315,7 +315,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -326,7 +326,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -338,7 +338,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -348,7 +348,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -380,7 +380,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -390,7 +390,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -401,7 +401,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -411,7 +411,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -422,7 +422,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -432,7 +432,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -443,7 +443,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -453,7 +453,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -489,36 +489,50 @@
 $ git branch master</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>Using Local File System as remote</t>
+  </si>
+  <si>
+    <t>Remote @ local</t>
+  </si>
+  <si>
+    <t>If you want to build a remote repo at local file system, use below command to build a remote repo:
+&gt; git init --bare /d/{repo_name}.git
+The you can add this as a remote origin (or whatever name) to your current git repo with below cmd:
+&gt; git remote add {origin_or_whatever} /d/{repo_name}.git
+And so that you can perform same feature to this "remote" just as github like clone/push/pull...
+p.s. For more information, refer to: http://www.thehorrors.org.uk/snippets/git-local-filesystem-remotes/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -526,21 +540,21 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="4"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -586,7 +600,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -599,7 +613,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -673,7 +687,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -708,7 +721,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -884,21 +896,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
-    <col min="2" max="2" width="17.25" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -909,7 +921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="38.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -920,7 +932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="51.75">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -931,7 +943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -942,7 +954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="141">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -953,7 +965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -964,7 +976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -975,7 +987,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -986,7 +998,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -997,7 +1009,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="26.25">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
@@ -1008,7 +1020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1019,7 +1031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="39">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -1030,7 +1042,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="39">
       <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
@@ -1041,7 +1053,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="26.25">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -1052,7 +1064,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="90">
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
@@ -1063,7 +1075,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="141">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -1074,7 +1086,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="111" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="102.75">
       <c r="A17" s="5" t="s">
         <v>45</v>
       </c>
@@ -1085,7 +1097,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="102.75">
       <c r="A18" s="5" t="s">
         <v>46</v>
       </c>
@@ -1096,7 +1108,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="90">
       <c r="A19" s="5" t="s">
         <v>46</v>
       </c>
@@ -1107,7 +1119,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="26.25">
       <c r="A20" s="5" t="s">
         <v>45</v>
       </c>
@@ -1118,117 +1130,123 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="102.75">
+      <c r="A21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3">
       <c r="A42" s="5"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3">
       <c r="A43" s="5"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3">
       <c r="A44" s="5"/>
     </row>
   </sheetData>
@@ -1239,12 +1257,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1252,12 +1270,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add git concept about submodule and staging area
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Language</t>
   </si>
@@ -503,12 +503,223 @@
 And so that you can perform same feature to this "remote" just as github like clone/push/pull...
 p.s. For more information, refer to: http://www.thehorrors.org.uk/snippets/git-local-filesystem-remotes/</t>
   </si>
+  <si>
+    <t>Git concept</t>
+  </si>
+  <si>
+    <t>Relationship between "working directory" and "staging area"</t>
+  </si>
+  <si>
+    <t>Git folder under git folder: submodule</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* When our new git folder contains another git folder, then the subfolder is name "submodule" in git machanism.
+* When do adding in parent git folder, submodule will present as {path}/{submodule_name} as a standalone item, then no details inside submodule will be revealed in the parent folder git console.
+* When submodule has some uncommited change (staged or not), the parent folder git status will note the changes in red item as below:
+    &gt; modified:   {path}/SUBMODULE1 (modified content, untracked content)
+    &gt; modified:   {path}/SUBMODULE2 (modified content)
+And user cannot stage above "changes" unless going inside submodule and clean the directory.
+(p.s. the error message when try to add the submodule in parent like: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Git: fatal: Pathspec is in submodule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> )</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">STAGE 本質上 is the product of comparasion between HEAD and WORKDIR. So items in STAGE can be regarded as " actions" basic on HEAD to become WORK. Below command or action is related:
+&gt; git add {…}      //move </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>red</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>green</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> entry in git status that add stuff to head
+&gt; git rm {…}       //move </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>red</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>green</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> entry in git status that remove stuffs from head
+&gt; git rm --cached {...}       //move </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>green</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>red</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to unstage
+&gt; git checkout -- {…}      //move </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>red</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to nth in git status
+&gt; user edit the WORK      //generate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>red</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> entry in git status</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,6 +765,21 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -900,7 +1126,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1141,15 +1367,27 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+    <row r="22" spans="1:3" ht="90">
+      <c r="A22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="141">
+      <c r="A23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="5"/>

</xml_diff>

<commit_message>
Add git entry on using stash, awesome tool
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <t>Language</t>
   </si>
@@ -713,6 +713,21 @@
       </rPr>
       <t xml:space="preserve"> entry in git status</t>
     </r>
+  </si>
+  <si>
+    <t>Git Stash</t>
+  </si>
+  <si>
+    <t>Working on master but need a quick reference to branch, stash can temp save the change and recover later on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save dirty workings on branch #1 
+&gt; git stash -u    //And now can switch to branch #2, while at this moment branch#1 status is clean 
+View Stash:
+&gt; git stash list
+Recover stash after switch back from branch#2:
+&gt; (at branch#1) git stash pop
+</t>
   </si>
 </sst>
 </file>
@@ -1125,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1389,10 +1404,16 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+    <row r="24" spans="1:3" ht="90">
+      <c r="A24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5"/>

</xml_diff>

<commit_message>
Add git log graph and show top n recent commit
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t>Language</t>
   </si>
@@ -721,13 +721,27 @@
     <t>Working on master but need a quick reference to branch, stash can temp save the change and recover later on</t>
   </si>
   <si>
-    <t xml:space="preserve">Save dirty workings on branch #1 
+    <t>Save dirty workings on branch #1 
 &gt; git stash -u    //And now can switch to branch #2, while at this moment branch#1 status is clean 
 View Stash:
 &gt; git stash list
 Recover stash after switch back from branch#2:
-&gt; (at branch#1) git stash pop
-</t>
+&gt; (at branch#1) git stash pop</t>
+  </si>
+  <si>
+    <t>Git Log</t>
+  </si>
+  <si>
+    <t>Present the graph</t>
+  </si>
+  <si>
+    <t>&gt;git log --oenline --decorate --graph</t>
+  </si>
+  <si>
+    <t>Show n recent commit</t>
+  </si>
+  <si>
+    <t>&gt;git log -n</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1155,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1404,7 +1418,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="90">
+    <row r="24" spans="1:3" ht="77.25">
       <c r="A24" s="5" t="s">
         <v>58</v>
       </c>
@@ -1416,14 +1430,26 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="A25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="26.25">
+      <c r="A26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="5"/>

</xml_diff>

<commit_message>
Add git log graph and add system property to java
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
   <si>
     <t>Language</t>
   </si>
@@ -742,6 +742,19 @@
   </si>
   <si>
     <t>&gt;git log -n</t>
+  </si>
+  <si>
+    <t>Git Ignore</t>
+  </si>
+  <si>
+    <t>git ignore system</t>
+  </si>
+  <si>
+    <t>1. Edit {home}/.git/info/exclude to ignore files, Every line regex the file that should (not) be ignored:
+# *.java    &lt;- ignore javas globally
+# !*.java  &lt;- don’t ignore java globally
+2. Put .gitignore file in any folder to state the ignore target in that folder.
+REF-- https://git-scm.com/docs/gitignore</t>
   </si>
 </sst>
 </file>
@@ -1155,7 +1168,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1451,10 +1464,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+    <row r="27" spans="1:3" ht="64.5">
+      <c r="A27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="5"/>

</xml_diff>

<commit_message>
Add git entry on gitignore
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>Language</t>
   </si>
@@ -755,6 +755,13 @@
 # !*.java  &lt;- don’t ignore java globally
 2. Put .gitignore file in any folder to state the ignore target in that folder.
 REF-- https://git-scm.com/docs/gitignore</t>
+  </si>
+  <si>
+    <t>git ignore system (2)</t>
+  </si>
+  <si>
+    <t>If some files are already under tracking, use below command to remove them from the working area:
+&gt; git rm --cached -r target        //recursively remove files under target folder</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1175,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1475,10 +1482,16 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+    <row r="28" spans="1:3" ht="26.25">
+      <c r="A28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="5"/>

</xml_diff>

<commit_message>
Add entry to git and maven lib
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -721,47 +721,48 @@
     <t>Working on master but need a quick reference to branch, stash can temp save the change and recover later on</t>
   </si>
   <si>
+    <t>Git Log</t>
+  </si>
+  <si>
+    <t>Present the graph</t>
+  </si>
+  <si>
+    <t>&gt;git log --oenline --decorate --graph</t>
+  </si>
+  <si>
+    <t>Show n recent commit</t>
+  </si>
+  <si>
+    <t>&gt;git log -n</t>
+  </si>
+  <si>
+    <t>Git Ignore</t>
+  </si>
+  <si>
+    <t>git ignore system</t>
+  </si>
+  <si>
+    <t>1. Edit {home}/.git/info/exclude to ignore files, Every line regex the file that should (not) be ignored:
+# *.java    &lt;- ignore javas globally
+# !*.java  &lt;- don’t ignore java globally
+2. Put .gitignore file in any folder to state the ignore target in that folder.
+REF-- https://git-scm.com/docs/gitignore</t>
+  </si>
+  <si>
+    <t>git ignore system (2)</t>
+  </si>
+  <si>
+    <t>If some files are already under tracking, use below command to remove them from the working area:
+&gt; git rm --cached -r target        //recursively remove files under target folder</t>
+  </si>
+  <si>
     <t>Save dirty workings on branch #1 
 &gt; git stash -u    //And now can switch to branch #2, while at this moment branch#1 status is clean 
 View Stash:
 &gt; git stash list
 Recover stash after switch back from branch#2:
-&gt; (at branch#1) git stash pop</t>
-  </si>
-  <si>
-    <t>Git Log</t>
-  </si>
-  <si>
-    <t>Present the graph</t>
-  </si>
-  <si>
-    <t>&gt;git log --oenline --decorate --graph</t>
-  </si>
-  <si>
-    <t>Show n recent commit</t>
-  </si>
-  <si>
-    <t>&gt;git log -n</t>
-  </si>
-  <si>
-    <t>Git Ignore</t>
-  </si>
-  <si>
-    <t>git ignore system</t>
-  </si>
-  <si>
-    <t>1. Edit {home}/.git/info/exclude to ignore files, Every line regex the file that should (not) be ignored:
-# *.java    &lt;- ignore javas globally
-# !*.java  &lt;- don’t ignore java globally
-2. Put .gitignore file in any folder to state the ignore target in that folder.
-REF-- https://git-scm.com/docs/gitignore</t>
-  </si>
-  <si>
-    <t>git ignore system (2)</t>
-  </si>
-  <si>
-    <t>If some files are already under tracking, use below command to remove them from the working area:
-&gt; git rm --cached -r target        //recursively remove files under target folder</t>
+&gt; (at branch#1) git stash pop
+** note: if stash doesnt cause confliction, it is transferable among different commit.</t>
   </si>
 </sst>
 </file>
@@ -1175,7 +1176,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1438,7 +1439,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="77.25">
+    <row r="24" spans="1:3" ht="90">
       <c r="A24" s="5" t="s">
         <v>58</v>
       </c>
@@ -1446,51 +1447,51 @@
         <v>59</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="26.25">
       <c r="A26" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="64.5">
       <c r="A27" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="26.25">
       <c r="A28" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3">

</xml_diff>

<commit_message>
Add git diff plugin info & python pip entry
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
   <si>
     <t>Language</t>
   </si>
@@ -763,6 +763,33 @@
 Recover stash after switch back from branch#2:
 &gt; (at branch#1) git stash pop
 ** note: if stash doesnt cause confliction, it is transferable among different commit.</t>
+  </si>
+  <si>
+    <t>Config系統</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>Extend git diff for excel</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>1. File ".gitignore" in a folder is equivalent to "/.git/info/exclude", the only difference is that former is only effective for local folder and latter is valid globally
+2. File ".gitattributes" and "/.git/info/attributes" and they are simular relationship like ignore files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add entry to  "/.git/info/attributes": 
+       $ *.xlsx diff=git_diff_xlsx
+2. Add entry to ".git/config":
+       $ [diff "git_diff_xlsx"]
+       $       binary = True
+       $       textconv = python C:/Users/BI77/Documents/playground/git_diff_xlsx.py
+3. Then when run git diff *.xlsx, git will use given command to generate difference.
+** Interesting fact noticed: git_diff_xlsx.py only need 1 file as input, and output stdin, so that I assume that git has its framework to compare 2 file stream. So by understanding this, I can develope my own plugin too!
+** The experiment git repo is the "Playground" folder in my BCM working directory </t>
   </si>
 </sst>
 </file>
@@ -861,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -872,6 +899,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1175,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1494,15 +1524,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+    <row r="29" spans="1:3" ht="39">
+      <c r="A29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="141">
+      <c r="A30" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="5"/>

</xml_diff>

<commit_message>
Add git entry on submodule
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>Language</t>
   </si>
@@ -790,6 +790,21 @@
 3. Then when run git diff *.xlsx, git will use given command to generate difference.
 ** Interesting fact noticed: git_diff_xlsx.py only need 1 file as input, and output stdin, so that I assume that git has its framework to compare 2 file stream. So by understanding this, I can develope my own plugin too!
 ** The experiment git repo is the "Playground" folder in my BCM working directory </t>
+  </si>
+  <si>
+    <t>Submodule</t>
+  </si>
+  <si>
+    <t>Submodule basic</t>
+  </si>
+  <si>
+    <t>When there is git under another git folder, the upper git will regard the deeper git as "Submodule". But not until in upper git invoke command: $ git submodule add {deeper_git} then the upper git will generate the .gitmodule file and start the management of the deeper git module.
+But the submodule's content will not commit to the upper git anyway. 
+Here are some usage:
+$ git submodule add /path/to/git/name.git
+$ git submodule status
+$ git submodule init
+$ git submodule deinit        // delete the git repo</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -1546,10 +1561,16 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+    <row r="31" spans="1:3" ht="115.5">
+      <c r="A31" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="5"/>

</xml_diff>

<commit_message>
1. Add java entry on springboot CommandLineRunner 2. Add git entry on browsing a file's history
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
   <si>
     <t>Language</t>
   </si>
@@ -805,6 +805,12 @@
 $ git submodule status
 $ git submodule init
 $ git submodule deinit        // delete the git repo</t>
+  </si>
+  <si>
+    <t>Browse a file history</t>
+  </si>
+  <si>
+    <t>$git log -p {filename}</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1227,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1572,10 +1578,16 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+    <row r="32" spans="1:3" ht="26.25">
+      <c r="A32" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="5"/>

</xml_diff>

<commit_message>
Add git entry on using liba as my own plugin, Add vim entry about set (no)wrap
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
   <si>
     <t>Language</t>
   </si>
@@ -841,6 +841,13 @@
     <t>Git introduced the worktree feature not too long ago (as of version 2.5, released July 2015). A great usage scenario can be found here: https://spin.atomicobject.com/2016/06/26/parallelize-development-git-worktrees/
 Set up worktree with below command:
 $ git worktree add ../new-worktree-dir some-existing-branch</t>
+  </si>
+  <si>
+    <t>Extend git diff for excel (2)</t>
+  </si>
+  <si>
+    <t>Previously we use python to parse an excel as git-diff's plugin. And now I try to use the liba.exe as the plugin and it works! Only need to change the textconv (in file .git/config) from previous setting:
+# textconv = ./liba -show</t>
   </si>
 </sst>
 </file>
@@ -1257,7 +1264,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1652,10 +1659,16 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+    <row r="36" spans="1:3" ht="39">
+      <c r="A36" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="5"/>

</xml_diff>

<commit_message>
Add markdwon language syntax
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
   <si>
     <t>Language</t>
   </si>
@@ -157,7 +157,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -167,7 +167,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -179,7 +179,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -189,7 +189,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -202,7 +202,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -213,7 +213,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -226,7 +226,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -236,7 +236,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -247,7 +247,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -257,7 +257,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -272,7 +272,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -282,7 +282,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -295,7 +295,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -306,7 +306,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -318,7 +318,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -328,7 +328,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -360,7 +360,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -370,7 +370,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -381,7 +381,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -391,7 +391,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -402,7 +402,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -412,7 +412,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -423,7 +423,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -433,7 +433,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -507,7 +507,7 @@
         <i/>
         <sz val="10"/>
         <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -517,7 +517,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -533,7 +533,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -543,7 +543,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -553,7 +553,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -563,7 +563,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -574,7 +574,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -584,7 +584,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -594,7 +594,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -604,7 +604,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -615,7 +615,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -625,7 +625,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -635,7 +635,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -645,7 +645,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -656,7 +656,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -666,7 +666,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -677,7 +677,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -687,7 +687,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -849,36 +849,144 @@
     <t>Previously we use python to parse an excel as git-diff's plugin. And now I try to use the liba.exe as the plugin and it works! Only need to change the textconv (in file .git/config) from previous setting:
 # textconv = ./liba -show</t>
   </si>
+  <si>
+    <t>Markdown</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intro</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">* Markdown is a markup language.
+* format extension: *.md
+* Github has the visualization tool. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Headers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t># This is an &lt;h1&gt; tag
+## This is an &lt;h2&gt; tag
+###### This is an &lt;h6&gt; tag</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emphasis</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>*This text will be italic*
+_This will also be italic_
+**This text will be bold**
+__This will also be bold__
+_You **can** combine them_</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lists Unordered</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* Item 1
+* Item 2
+  * Item 2a
+  * Item 2b</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Item 1
+1. Item 2
+1. Item 3
+   1. Item 3a
+   1. Item 3b</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lists ordered</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Images</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>![GitHub Logo](/images/logo.png)
+Format: ![Alt Text](url)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Links</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://github.com - automatic!
+[GitHub](http://github.com)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blockquotes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>As Kanye West said:
+&gt; We're living the future so
+&gt; the present is our past.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inline code</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>I think you should use an
+`&lt;addr&gt;` element here instead.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>```javascript
+if (isAwesome){
+  return true
+}
+```</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code with Language Declare</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -886,21 +994,21 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="4"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -908,14 +1016,14 @@
       <i/>
       <sz val="10"/>
       <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -946,7 +1054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -962,9 +1070,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -977,7 +1088,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1051,6 +1162,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1085,6 +1197,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1260,21 +1373,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="17.25" customWidth="1"/>
     <col min="3" max="3" width="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1285,7 +1398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="38.25">
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1296,7 +1409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="51.75">
+    <row r="3" spans="1:3" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1307,7 +1420,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1318,7 +1431,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="141">
+    <row r="5" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1329,7 +1442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>85</v>
       </c>
@@ -1340,7 +1453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>85</v>
       </c>
@@ -1351,7 +1464,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>85</v>
       </c>
@@ -1362,7 +1475,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>85</v>
       </c>
@@ -1373,7 +1486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="26.25">
+    <row r="10" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>84</v>
       </c>
@@ -1384,7 +1497,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
@@ -1395,7 +1508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="39">
+    <row r="12" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>82</v>
       </c>
@@ -1406,7 +1519,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="39">
+    <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>83</v>
       </c>
@@ -1417,7 +1530,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="26.25">
+    <row r="14" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>83</v>
       </c>
@@ -1428,7 +1541,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="90">
+    <row r="15" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
@@ -1439,7 +1552,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="141">
+    <row r="16" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>86</v>
       </c>
@@ -1450,7 +1563,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="102.75">
+    <row r="17" spans="1:3" ht="111" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>86</v>
       </c>
@@ -1461,7 +1574,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="102.75">
+    <row r="18" spans="1:3" ht="111" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
@@ -1472,7 +1585,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="90">
+    <row r="19" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>41</v>
       </c>
@@ -1483,7 +1596,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="26.25">
+    <row r="20" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
@@ -1494,7 +1607,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="102.75">
+    <row r="21" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
@@ -1505,7 +1618,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="90">
+    <row r="22" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>48</v>
       </c>
@@ -1516,7 +1629,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="141">
+    <row r="23" spans="1:3" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>48</v>
       </c>
@@ -1527,7 +1640,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="90">
+    <row r="24" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>87</v>
       </c>
@@ -1538,7 +1651,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>81</v>
       </c>
@@ -1549,7 +1662,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="26.25">
+    <row r="26" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>81</v>
       </c>
@@ -1560,7 +1673,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="64.5">
+    <row r="27" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>58</v>
       </c>
@@ -1571,7 +1684,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="26.25">
+    <row r="28" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>58</v>
       </c>
@@ -1582,7 +1695,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="39">
+    <row r="29" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>64</v>
       </c>
@@ -1593,7 +1706,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="141">
+    <row r="30" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>65</v>
       </c>
@@ -1604,7 +1717,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="115.5">
+    <row r="31" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>70</v>
       </c>
@@ -1615,7 +1728,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="26.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>65</v>
       </c>
@@ -1626,7 +1739,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="102.75">
+    <row r="33" spans="1:3" ht="111" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>75</v>
       </c>
@@ -1637,7 +1750,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="64.5">
+    <row r="34" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>79</v>
       </c>
@@ -1648,7 +1761,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="64.5">
+    <row r="35" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>78</v>
       </c>
@@ -1659,7 +1772,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="39">
+    <row r="36" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>65</v>
       </c>
@@ -1670,53 +1783,130 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="5"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="5"/>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="5"/>
+    <row r="37" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1724,12 +1914,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add git entry on line ending handling in cross-OS project
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="116">
   <si>
     <t>Language</t>
   </si>
@@ -157,7 +157,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -167,7 +167,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -179,7 +179,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -189,7 +189,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -202,7 +202,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -213,7 +213,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -226,7 +226,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -236,7 +236,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -247,7 +247,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -257,7 +257,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -272,7 +272,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -282,7 +282,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -295,7 +295,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="4"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -306,7 +306,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -318,7 +318,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -328,7 +328,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -360,7 +360,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -370,7 +370,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -381,7 +381,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -391,7 +391,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -402,7 +402,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -412,7 +412,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -423,7 +423,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -433,7 +433,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -507,7 +507,7 @@
         <i/>
         <sz val="10"/>
         <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -517,7 +517,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -533,7 +533,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -543,7 +543,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -553,7 +553,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FF00B050"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -563,7 +563,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -574,7 +574,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -584,7 +584,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -594,7 +594,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FF00B050"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -604,7 +604,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -615,7 +615,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FF00B050"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -625,7 +625,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -635,7 +635,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -645,7 +645,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -656,7 +656,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -666,7 +666,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -677,7 +677,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -687,7 +687,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -957,36 +957,66 @@
     <t>Code with Language Declare</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>git</t>
+  </si>
+  <si>
+    <t>line ending</t>
+  </si>
+  <si>
+    <t># Handling line ending in cross-OS git project
+## Background
+Previously when I am exploring the vim plugin, I ran into the line-end problem the first time. I used vim to set file format to unix and solve adhoc fix. But later it appears that after resetup of cygwin on windows, it regards all file as different version in git due to the line end conflict. Then I try to look for a solution from git.
+## Solution of git 
+It provides a git attribute setting that ensure cross OS project align the line ends. Here is how it works:
+* __Set in .gitattributes__ 
+```
+# Set the default behavior, in case people don't have core.autocrlf set.
+* text=auto
+# Explicitly declare text files you want to always be normalized and converted
+# to native line endings on checkout.
+*.c text
+*.h text
+# Declare files that will always have CRLF line endings on checkout.
+*.sln text eol=crlf
+# Denote all files that are truly binary and should not be modified.
+*.png binary
+*.jpg binary
+```
+* __Set in global setting for a linux machine__ `git config --global core.autocrlf input`
+* __Set in global setting for a win machine__ `git config --global core.autocrlf true`
+&gt; ref: https://help.github.com/articles/dealing-with-line-endings/#platform-all</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -994,21 +1024,21 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="4"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1016,14 +1046,14 @@
       <i/>
       <sz val="10"/>
       <color theme="0" tint="-0.499984740745262"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF00B050"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1075,7 +1105,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1088,7 +1118,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1162,7 +1192,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1197,7 +1226,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1373,21 +1401,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:A46"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
-    <col min="2" max="2" width="17.25" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1398,7 +1426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="38.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1409,7 +1437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="51.75">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1420,7 +1448,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1431,7 +1459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="141">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1442,7 +1470,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
         <v>85</v>
       </c>
@@ -1453,7 +1481,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
         <v>85</v>
       </c>
@@ -1464,7 +1492,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
         <v>85</v>
       </c>
@@ -1475,7 +1503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
         <v>85</v>
       </c>
@@ -1486,7 +1514,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="26.25">
       <c r="A10" s="5" t="s">
         <v>84</v>
       </c>
@@ -1497,7 +1525,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
@@ -1508,7 +1536,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="39">
       <c r="A12" s="5" t="s">
         <v>82</v>
       </c>
@@ -1519,7 +1547,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="39">
       <c r="A13" s="5" t="s">
         <v>83</v>
       </c>
@@ -1530,7 +1558,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="26.25">
       <c r="A14" s="5" t="s">
         <v>83</v>
       </c>
@@ -1541,7 +1569,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="90">
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
@@ -1552,7 +1580,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="141">
       <c r="A16" s="4" t="s">
         <v>86</v>
       </c>
@@ -1563,7 +1591,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="111" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="102.75">
       <c r="A17" s="5" t="s">
         <v>86</v>
       </c>
@@ -1574,7 +1602,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="111" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="102.75">
       <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
@@ -1585,7 +1613,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="90">
       <c r="A19" s="5" t="s">
         <v>41</v>
       </c>
@@ -1596,7 +1624,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="26.25">
       <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
@@ -1607,7 +1635,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="102.75">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
@@ -1618,7 +1646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="90">
       <c r="A22" s="5" t="s">
         <v>48</v>
       </c>
@@ -1629,7 +1657,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="141">
       <c r="A23" s="5" t="s">
         <v>48</v>
       </c>
@@ -1640,7 +1668,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="90">
       <c r="A24" s="5" t="s">
         <v>87</v>
       </c>
@@ -1651,7 +1679,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
         <v>81</v>
       </c>
@@ -1662,7 +1690,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="26.25">
       <c r="A26" s="5" t="s">
         <v>81</v>
       </c>
@@ -1673,7 +1701,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="64.5">
       <c r="A27" s="5" t="s">
         <v>58</v>
       </c>
@@ -1684,7 +1712,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="26.25">
       <c r="A28" s="5" t="s">
         <v>58</v>
       </c>
@@ -1695,7 +1723,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="39">
       <c r="A29" s="5" t="s">
         <v>64</v>
       </c>
@@ -1706,7 +1734,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="152.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="141">
       <c r="A30" s="5" t="s">
         <v>65</v>
       </c>
@@ -1717,7 +1745,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="115.5">
       <c r="A31" s="5" t="s">
         <v>70</v>
       </c>
@@ -1728,7 +1756,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="26.25">
       <c r="A32" s="5" t="s">
         <v>65</v>
       </c>
@@ -1739,7 +1767,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="111" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="102.75">
       <c r="A33" s="5" t="s">
         <v>75</v>
       </c>
@@ -1750,7 +1778,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="64.5">
       <c r="A34" s="5" t="s">
         <v>79</v>
       </c>
@@ -1761,7 +1789,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="64.5">
       <c r="A35" s="5" t="s">
         <v>78</v>
       </c>
@@ -1772,7 +1800,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="39">
       <c r="A36" s="5" t="s">
         <v>65</v>
       </c>
@@ -1783,7 +1811,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="39">
       <c r="A37" s="5" t="s">
         <v>92</v>
       </c>
@@ -1794,7 +1822,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="39">
       <c r="A38" s="5" t="s">
         <v>92</v>
       </c>
@@ -1805,7 +1833,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="90">
       <c r="A39" s="5" t="s">
         <v>92</v>
       </c>
@@ -1816,7 +1844,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="51.75">
       <c r="A40" s="5" t="s">
         <v>92</v>
       </c>
@@ -1827,7 +1855,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="75">
       <c r="A41" s="5" t="s">
         <v>92</v>
       </c>
@@ -1838,7 +1866,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="30">
       <c r="A42" s="5" t="s">
         <v>92</v>
       </c>
@@ -1849,7 +1877,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="30">
       <c r="A43" s="5" t="s">
         <v>92</v>
       </c>
@@ -1860,7 +1888,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="60">
       <c r="A44" s="5" t="s">
         <v>92</v>
       </c>
@@ -1871,7 +1899,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="30">
       <c r="A45" s="5" t="s">
         <v>92</v>
       </c>
@@ -1882,7 +1910,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="75">
       <c r="A46" s="5" t="s">
         <v>92</v>
       </c>
@@ -1891,6 +1919,17 @@
       </c>
       <c r="C46" s="7" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="92.25" customHeight="1">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>114</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1901,12 +1940,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1914,12 +1953,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add git entry on building git server
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="119">
   <si>
     <t>Language</t>
   </si>
@@ -986,6 +986,22 @@
 * __Set in global setting for a linux machine__ `git config --global core.autocrlf input`
 * __Set in global setting for a win machine__ `git config --global core.autocrlf true`
 &gt; ref: https://help.github.com/articles/dealing-with-line-endings/#platform-all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote </t>
+  </si>
+  <si>
+    <t>My own git server</t>
+  </si>
+  <si>
+    <t># Different Ways to Host Git Server
+* Local Protocol: Local File System / Network File System
+* SSH Protocol
+* Http Protocol
+* Git Protocol
+# Use Local Protocol
+* Clone existing project to build: `git clone --bare my_project my_project.git`
+* Init an Empty project git: `git init --bare new_project.git`</t>
   </si>
 </sst>
 </file>
@@ -1402,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1930,6 +1946,17 @@
       </c>
       <c r="C47" s="7" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="120">
+      <c r="A48" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove markdown entry from git lib
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
   <si>
     <t>Language</t>
   </si>
@@ -848,114 +848,6 @@
   <si>
     <t>Previously we use python to parse an excel as git-diff's plugin. And now I try to use the liba.exe as the plugin and it works! Only need to change the textconv (in file .git/config) from previous setting:
 # textconv = ./liba -show</t>
-  </si>
-  <si>
-    <t>Markdown</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intro</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">* Markdown is a markup language.
-* format extension: *.md
-* Github has the visualization tool. </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Headers</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t># This is an &lt;h1&gt; tag
-## This is an &lt;h2&gt; tag
-###### This is an &lt;h6&gt; tag</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emphasis</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>*This text will be italic*
-_This will also be italic_
-**This text will be bold**
-__This will also be bold__
-_You **can** combine them_</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lists Unordered</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* Item 1
-* Item 2
-  * Item 2a
-  * Item 2b</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Item 1
-1. Item 2
-1. Item 3
-   1. Item 3a
-   1. Item 3b</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lists ordered</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Images</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>![GitHub Logo](/images/logo.png)
-Format: ![Alt Text](url)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Links</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://github.com - automatic!
-[GitHub](http://github.com)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Blockquotes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>As Kanye West said:
-&gt; We're living the future so
-&gt; the present is our past.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inline code</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>I think you should use an
-`&lt;addr&gt;` element here instead.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>```javascript
-if (isAwesome){
-  return true
-}
-```</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Code with Language Declare</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>git</t>
@@ -1418,10 +1310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1827,138 +1719,29 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="39">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:3" ht="174.75" customHeight="1">
+      <c r="A37" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="39">
-      <c r="A38" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" s="5" t="s">
+    <row r="38" spans="1:3" ht="120">
+      <c r="A38" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="B38" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="90">
-      <c r="A39" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B39" s="5" t="s">
+      <c r="C38" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="51.75">
-      <c r="A40" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="75">
-      <c r="A41" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="30">
-      <c r="A42" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="30">
-      <c r="A43" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="60">
-      <c r="A44" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="30">
-      <c r="A45" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="75">
-      <c r="A46" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="92.25" customHeight="1">
-      <c r="A47" t="s">
-        <v>113</v>
-      </c>
-      <c r="B47" t="s">
-        <v>114</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="120">
-      <c r="A48" t="s">
-        <v>116</v>
-      </c>
-      <c r="B48" t="s">
-        <v>117</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
+    </row>
+    <row r="47" spans="1:3" ht="92.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add git entry about tagging
</commit_message>
<xml_diff>
--- a/git_lib.xlsx
+++ b/git_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="101">
   <si>
     <t>Language</t>
   </si>
@@ -894,6 +894,21 @@
 # Use Local Protocol
 * Clone existing project to build: `git clone --bare my_project my_project.git`
 * Init an Empty project git: `git init --bare new_project.git`</t>
+  </si>
+  <si>
+    <t>Tagging</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t># Basic command
+`git tag ` //show all tags (both lightweight and annotated)
+`git tag v1.1` //lightweight tag HEAD to v1.1
+`git tag -a v1.4 -m "my version 1.4"` //build annotated tag v1.4
+`git show v1.1` //show the diff between v1.1 and previous commit
+# Concept
+There are 2 kinds of tags, lightweight and Annotated. Lightweight tag is like a final branch. Annotated tag is a copy in object tree and might go with key and signature and blablabla.</t>
   </si>
 </sst>
 </file>
@@ -1312,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1739,6 +1754,17 @@
       </c>
       <c r="C38" s="7" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="120">
+      <c r="A39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="92.25" customHeight="1"/>

</xml_diff>